<commit_message>
28 June 2025 Dorm
</commit_message>
<xml_diff>
--- a/ESP32-C3-PHILS/BOM.xlsx
+++ b/ESP32-C3-PHILS/BOM.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\develop\Altium\ESP32-C3-PHILS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium Files\altiumprojects\ESP32-C3-PHILS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B74E0EF-854B-4755-81E7-A3CE56050EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D2984450-487D-4152-8B99-D03DAA8A836E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23750" windowHeight="12030"/>
   </bookViews>
   <sheets>
-    <sheet name="nbuxy3cb" sheetId="1" r:id="rId1"/>
+    <sheet name="yzvtsanc" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">nbuxy3cb!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">yzvtsanc!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="161">
   <si>
     <t>Description</t>
   </si>
@@ -45,12 +44,12 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>Manufacturer Part Number</t>
   </si>
   <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
     <t>Chip Dielectric Antenna; 1dBi; 2450MHz; T/R | Abracon AMCA31-2R450G-S1F-T3</t>
   </si>
   <si>
@@ -63,7 +62,7 @@
     <t>AMCA31-2R450G-S1F-T3</t>
   </si>
   <si>
-    <t>ANT</t>
+    <t>Abracon</t>
   </si>
   <si>
     <t>connector, rf coaxial, sma str jack for p.c.board, 4 legs, .050 center cont, 50 ohm</t>
@@ -78,6 +77,9 @@
     <t>132134</t>
   </si>
   <si>
+    <t>Amphenol Connex</t>
+  </si>
+  <si>
     <t>Multilayer Ceramic Capacitor, 0.1 uF, 16 V, ï¿½ 10%, X7R, 0402 [1005 Metric]</t>
   </si>
   <si>
@@ -90,7 +92,7 @@
     <t>CC0402KRX7R7BB104</t>
   </si>
   <si>
-    <t>104</t>
+    <t>Yageo</t>
   </si>
   <si>
     <t>Multilayer Ceramic Chip Capacitor 0402 Size 10uF 10V X5R ±20% Tolerance SMD T/R</t>
@@ -105,15 +107,12 @@
     <t>0402ZD106MAT2A</t>
   </si>
   <si>
-    <t>C106</t>
+    <t>Kyocera AVX</t>
   </si>
   <si>
     <t>C5, C14, C30</t>
   </si>
   <si>
-    <t>106</t>
-  </si>
-  <si>
     <t>Multilayer Ceramic Capacitor, 2.2 uF, 6.3 V, ï¿½ 20%, X5R, 0402 [1005 Metric]</t>
   </si>
   <si>
@@ -129,6 +128,9 @@
     <t>CL05A225MQ5NNNC</t>
   </si>
   <si>
+    <t>Samsung</t>
+  </si>
+  <si>
     <t>0402 10 pF 50 V ±5 % Tolerance NP0 SMT Multilayer Ceramic Capacitor</t>
   </si>
   <si>
@@ -138,9 +140,6 @@
     <t>C10</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>CC0402JRNPO9BN100</t>
   </si>
   <si>
@@ -159,6 +158,9 @@
     <t>GRM0335C1E3R3BA01D</t>
   </si>
   <si>
+    <t>Murata</t>
+  </si>
+  <si>
     <t>Single Color LED, Ultra Bright Orange, Water Clear, 1.1mm</t>
   </si>
   <si>
@@ -171,12 +173,21 @@
     <t>LTST-C190KFKT</t>
   </si>
   <si>
-    <t>LED</t>
+    <t>Vishay Lite-On</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>J1, J3</t>
+  </si>
+  <si>
+    <t>HEADERPAD_20_80MIL</t>
+  </si>
+  <si>
+    <t>PH2-20-UA</t>
+  </si>
+  <si>
     <t>USB Connector, 16 Contact(s), Male, Right Angle, Surface Mount Terminal, Locking, Receptacle</t>
   </si>
   <si>
@@ -189,7 +200,7 @@
     <t>USB4110-GF-A</t>
   </si>
   <si>
-    <t>USB-C</t>
+    <t>Global Connector Technology</t>
   </si>
   <si>
     <t>Conn Unshrouded Header HDR 6 POS 2.54mm Solder ST Top Entry SMD C-Grid Bag</t>
@@ -204,6 +215,9 @@
     <t>15-91-0060</t>
   </si>
   <si>
+    <t>Molex</t>
+  </si>
+  <si>
     <t>Conn Unshrouded Header HDR 40 POS 2.54mm Solder ST Top Entry SMD Bulk</t>
   </si>
   <si>
@@ -219,6 +233,9 @@
     <t>95157-440LF</t>
   </si>
   <si>
+    <t>Amphenol ICC / FCI</t>
+  </si>
+  <si>
     <t>Inductor with Inductance: 2.2nH Tol. +/-0.1nH, Package: 0402 (1005)</t>
   </si>
   <si>
@@ -246,6 +263,9 @@
     <t>SPH252010H2R2MT</t>
   </si>
   <si>
+    <t>Sunlord</t>
+  </si>
+  <si>
     <t>Inductor High Frequency Chip Unshielded Multi-Layer 2.2nH 0.1nH 500MHz 14Q-Factor Ceramic 600mA 100mOhm DCR 0201 T/R</t>
   </si>
   <si>
@@ -258,7 +278,7 @@
     <t>MLG0603P2N2BT000</t>
   </si>
   <si>
-    <t>2n2</t>
+    <t>TDK</t>
   </si>
   <si>
     <t>SMD Chip Resistor, 5.1 kOhm, ï¿½ 1%, 62.5 mW, 0402 [1005 Metric], Thick Film, General Purpose</t>
@@ -270,9 +290,6 @@
     <t>RC0402FR-075K1L</t>
   </si>
   <si>
-    <t>5K1</t>
-  </si>
-  <si>
     <t>Res Thin Film 0402 2K Ohm 0.1% 0.063W ±25ppm/°C Molded SMD Punched Carrier T/R</t>
   </si>
   <si>
@@ -285,6 +302,9 @@
     <t>ERA-2AEB202X</t>
   </si>
   <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
     <t>Res Thin Film 0402 15K Ohm 0.1% 0.063W(1/16W) ±25ppm/C Pad SMD T/R</t>
   </si>
   <si>
@@ -324,6 +344,21 @@
     <t>SKRKAHE020</t>
   </si>
   <si>
+    <t>Alps Electric</t>
+  </si>
+  <si>
+    <t>T1, T2, T4, T17, T18</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>T3, T5, T6, T7, T8, T9, T10, T11, T12, T13, T14, T15, T16, T19, T20, T21</t>
+  </si>
+  <si>
+    <t>JumpA</t>
+  </si>
+  <si>
     <t>ESD Suppressor Diode Array Dual Uni-Dir 15kV Air Gap/15kV Contact Disc 6-Pin SOT-23 T/R</t>
   </si>
   <si>
@@ -336,7 +371,7 @@
     <t>USBLC6-2SC6</t>
   </si>
   <si>
-    <t>USBLC6</t>
+    <t>STMicroelectronics</t>
   </si>
   <si>
     <t>Linear Voltage Regulator IC Positive Fixed 1 Output 500mA SOT-23-5</t>
@@ -472,9 +507,6 @@
   </si>
   <si>
     <t>ECS-400-18-33-JGN-TR3</t>
-  </si>
-  <si>
-    <t>CRYSTAL 40.0000MHZ 18PF SMD</t>
   </si>
   <si>
     <t>50-ECS-400-18-33-JGN-TR3TR-ND</t>
@@ -483,21 +515,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -540,26 +564,14 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +606,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -606,7 +618,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -653,23 +665,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -705,23 +700,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -873,24 +851,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E454E0D-334E-4A37-B306-EB03B4A4E2DE}">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="161.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" customWidth="1"/>
-    <col min="3" max="3" width="26.796875" customWidth="1"/>
-    <col min="4" max="5" width="17.296875" customWidth="1"/>
-    <col min="6" max="6" width="26.09765625" customWidth="1"/>
-    <col min="7" max="7" width="31.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="29.26953125" customWidth="1"/>
+    <col min="4" max="5" width="18.81640625" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -913,7 +891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -930,13 +908,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -953,24 +931,24 @@
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>17</v>
@@ -979,21 +957,21 @@
         <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -1002,33 +980,33 @@
         <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1045,36 +1023,36 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -1094,21 +1072,21 @@
         <v>42</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1117,10 +1095,10 @@
         <v>47</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -1134,24 +1112,20 @@
         <v>52</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>56</v>
@@ -1166,7 +1140,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -1177,7 +1151,7 @@
         <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1189,7 +1163,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -1206,222 +1180,216 @@
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1">
         <v>2</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="F17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="1">
         <v>8</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>108</v>
@@ -1430,205 +1398,251 @@
         <v>109</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="1">
+        <v>16</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E31" s="1">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="C33" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
15.02 july 2025 office
</commit_message>
<xml_diff>
--- a/ESP32-C3-PHILS/BOM.xlsx
+++ b/ESP32-C3-PHILS/BOM.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Altium Files\altiumprojects\ESP32-C3-PHILS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanion-012\altiums\altiumprojects\ESP32-C3-PHILS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23750" windowHeight="12030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10488"/>
   </bookViews>
   <sheets>
-    <sheet name="yzvtsanc" sheetId="1" r:id="rId1"/>
+    <sheet name="spdkf1cm" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">yzvtsanc!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">spdkf1cm!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
   <si>
     <t>Description</t>
   </si>
@@ -62,6 +62,9 @@
     <t>AMCA31-2R450G-S1F-T3</t>
   </si>
   <si>
+    <t>C3283994</t>
+  </si>
+  <si>
     <t>Abracon</t>
   </si>
   <si>
@@ -74,7 +77,7 @@
     <t>SMA_VERTICAL</t>
   </si>
   <si>
-    <t>132134</t>
+    <t>C3174425</t>
   </si>
   <si>
     <t>Amphenol Connex</t>
@@ -83,7 +86,7 @@
     <t>Multilayer Ceramic Capacitor, 0.1 uF, 16 V, ï¿½ 10%, X7R, 0402 [1005 Metric]</t>
   </si>
   <si>
-    <t>C1, C2, C4, C6, C7, C8, C9, C10, C11, C12, C13, C15, C17, C18, C21, C22, C29</t>
+    <t>C1, C2, C4, C6, C7, C9, C10, C11, C12, C13, C15, C17, C18, C21, C22, C29</t>
   </si>
   <si>
     <t>CAPC1005X55N2</t>
@@ -107,6 +110,9 @@
     <t>0402ZD106MAT2A</t>
   </si>
   <si>
+    <t>C2167902</t>
+  </si>
+  <si>
     <t>Kyocera AVX</t>
   </si>
   <si>
@@ -143,22 +149,16 @@
     <t>CC0402JRNPO9BN100</t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitor, 3.3 pF, 25 V, ± 0.1pF, C0G (NP0), 0201 [0603 Metric]</t>
+    <t>Ceramic Capacitor, Multilayer, Ceramic, 200V, 3.0304% +Tol, 3.0304% -Tol, C0G, 30ppm/Cel TC, 0.0000033uF, Surface...</t>
   </si>
   <si>
     <t>C25, C26, C27, C28</t>
   </si>
   <si>
-    <t>CAPC0603X33N</t>
-  </si>
-  <si>
-    <t>3.3PF0201</t>
-  </si>
-  <si>
-    <t>GRM0335C1E3R3BA01D</t>
-  </si>
-  <si>
-    <t>Murata</t>
+    <t>3.3PF0402</t>
+  </si>
+  <si>
+    <t>600L3R3BT200T4K</t>
   </si>
   <si>
     <t>Single Color LED, Ultra Bright Orange, Water Clear, 1.1mm</t>
@@ -173,6 +173,9 @@
     <t>LTST-C190KFKT</t>
   </si>
   <si>
+    <t>C157740</t>
+  </si>
+  <si>
     <t>Vishay Lite-On</t>
   </si>
   <si>
@@ -200,6 +203,9 @@
     <t>USB4110-GF-A</t>
   </si>
   <si>
+    <t>C5143397</t>
+  </si>
+  <si>
     <t>Global Connector Technology</t>
   </si>
   <si>
@@ -212,7 +218,7 @@
     <t>HEADER6PIN2.54</t>
   </si>
   <si>
-    <t>15-91-0060</t>
+    <t>C586557</t>
   </si>
   <si>
     <t>Molex</t>
@@ -230,7 +236,7 @@
     <t>HEADER_40PIN_SMD</t>
   </si>
   <si>
-    <t>95157-440LF</t>
+    <t>C5411221</t>
   </si>
   <si>
     <t>Amphenol ICC / FCI</t>
@@ -239,7 +245,7 @@
     <t>Inductor with Inductance: 2.2nH Tol. +/-0.1nH, Package: 0402 (1005)</t>
   </si>
   <si>
-    <t>L1</t>
+    <t>L1, L3, L4</t>
   </si>
   <si>
     <t>INDC1006X60N</t>
@@ -248,7 +254,7 @@
     <t>IND2n2</t>
   </si>
   <si>
-    <t>LQW15AN2N2B80D</t>
+    <t>LQW15AN2N2B80D, C2041833</t>
   </si>
   <si>
     <t>Fixed Ind 2.220%UH 0.114 Ohm 1800</t>
@@ -263,24 +269,12 @@
     <t>SPH252010H2R2MT</t>
   </si>
   <si>
+    <t>C5664568</t>
+  </si>
+  <si>
     <t>Sunlord</t>
   </si>
   <si>
-    <t>Inductor High Frequency Chip Unshielded Multi-Layer 2.2nH 0.1nH 500MHz 14Q-Factor Ceramic 600mA 100mOhm DCR 0201 T/R</t>
-  </si>
-  <si>
-    <t>L3, L4</t>
-  </si>
-  <si>
-    <t>INDC0603X33N</t>
-  </si>
-  <si>
-    <t>MLG0603P2N2BT000</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
     <t>SMD Chip Resistor, 5.1 kOhm, ï¿½ 1%, 62.5 mW, 0402 [1005 Metric], Thick Film, General Purpose</t>
   </si>
   <si>
@@ -290,6 +284,9 @@
     <t>RC0402FR-075K1L</t>
   </si>
   <si>
+    <t>C105872</t>
+  </si>
+  <si>
     <t>Res Thin Film 0402 2K Ohm 0.1% 0.063W ±25ppm/°C Molded SMD Punched Carrier T/R</t>
   </si>
   <si>
@@ -299,7 +296,7 @@
     <t>2K2</t>
   </si>
   <si>
-    <t>ERA-2AEB202X</t>
+    <t>ERA2AEB202X</t>
   </si>
   <si>
     <t>Panasonic</t>
@@ -314,7 +311,7 @@
     <t>15K0402</t>
   </si>
   <si>
-    <t>RT0402BRD0715KL</t>
+    <t>C852545</t>
   </si>
   <si>
     <t>SMD Chip Resistor, 33 Kohm, ½ 5%, 62.5 Mw, 0402 [1005 Metric], Thick Film, General Purpose</t>
@@ -341,13 +338,13 @@
     <t>SW_P</t>
   </si>
   <si>
-    <t>SKRKAHE020</t>
+    <t>C202388</t>
   </si>
   <si>
     <t>Alps Electric</t>
   </si>
   <si>
-    <t>T1, T2, T4, T17, T18</t>
+    <t>T1, T2, T4</t>
   </si>
   <si>
     <t>TP</t>
@@ -371,6 +368,9 @@
     <t>USBLC6-2SC6</t>
   </si>
   <si>
+    <t>C7519</t>
+  </si>
+  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
@@ -386,6 +386,9 @@
     <t>SPX3819M5-L-3-3</t>
   </si>
   <si>
+    <t>C9055</t>
+  </si>
+  <si>
     <t>WiFi Modules (802.11) (Engineering Samples Only) SMD IC ESP32-C3, RISC-V single-core MCU, 2.4G Wi-Fi &amp; BLE 5.0 combo, QFN 32-pin, 5*5 mm, 40 ~ 105C</t>
   </si>
   <si>
@@ -398,7 +401,7 @@
     <t>ESP32-C3</t>
   </si>
   <si>
-    <t>1904-ESP32-C3TR-ND</t>
+    <t>C2838500</t>
   </si>
   <si>
     <t>High-performance 6-axis inertial sensor (accelerometer + gyroscope) &lt;a href="https://pricing.snapeda.com/parts/BMI088/Bosch%20Sensortec/view-part?ref=eda"&gt;Check prices&lt;/a&gt;</t>
@@ -413,7 +416,7 @@
     <t>BMI088</t>
   </si>
   <si>
-    <t>828-1082-2-ND</t>
+    <t>C194919</t>
   </si>
   <si>
     <t>No Description Available</t>
@@ -428,7 +431,7 @@
     <t>BMM350</t>
   </si>
   <si>
-    <t>828-BMM350TR-ND</t>
+    <t>C17225907</t>
   </si>
   <si>
     <t>NOR Flash Serial (SPI, Dual SPI, Quad SPI) 3V/3.3V 16M-bit 2M x 8 6ns 8-Pin USON EP T/R</t>
@@ -443,7 +446,7 @@
     <t>W25Q16JVUXIQ_TR</t>
   </si>
   <si>
-    <t>W25Q16JVUXIQ TR</t>
+    <t>C2843335</t>
   </si>
   <si>
     <t>Gas sensor measuring relative humidity, barometric pressure, ambient temperature and gas (VOC)</t>
@@ -458,7 +461,7 @@
     <t>BME688</t>
   </si>
   <si>
-    <t>828-BME688TR-ND</t>
+    <t>C3664478</t>
   </si>
   <si>
     <t>U8</t>
@@ -470,7 +473,7 @@
     <t>BMP390</t>
   </si>
   <si>
-    <t>828-BMP390TR-ND</t>
+    <t>C2684802</t>
   </si>
   <si>
     <t>Digital Relative Humidity Temperature Sensor, Â±1.0 %RH, Â±0.1 Â°C, Ultra-Low-Power, with filtermembrane</t>
@@ -485,9 +488,6 @@
     <t>SHT45-AD1B-R3</t>
   </si>
   <si>
-    <t>1649-SHT45-AD1B-R3TR-ND</t>
-  </si>
-  <si>
     <t>GNSS Module Dual-Band 3V to 3.63V 18-Pin LCC T/R</t>
   </si>
   <si>
@@ -500,6 +500,9 @@
     <t>TESEO-LIV4FTR</t>
   </si>
   <si>
+    <t>C6284698</t>
+  </si>
+  <si>
     <t>Y1</t>
   </si>
   <si>
@@ -509,19 +512,27 @@
     <t>ECS-400-18-33-JGN-TR3</t>
   </si>
   <si>
-    <t>50-ECS-400-18-33-JGN-TR3TR-ND</t>
+    <t>C6239277</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -564,17 +575,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -590,7 +613,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -852,23 +875,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
-    <col min="3" max="3" width="29.26953125" customWidth="1"/>
-    <col min="4" max="5" width="18.81640625" customWidth="1"/>
-    <col min="6" max="6" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="17.796875" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" customWidth="1"/>
+    <col min="3" max="3" width="26.796875" customWidth="1"/>
+    <col min="4" max="5" width="17.296875" customWidth="1"/>
+    <col min="6" max="6" width="30.09765625" customWidth="1"/>
+    <col min="7" max="7" width="28.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -891,7 +914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -908,174 +931,174 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1">
-        <v>17</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1">
         <v>4</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1092,24 +1115,24 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -1117,532 +1140,510 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E17" s="1">
+        <v>8</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="1">
         <v>2</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="1">
-        <v>8</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E23" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E24" s="1">
-        <v>16</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E31" s="1">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>153</v>
+        <v>50</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G35" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="G34" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>